<commit_message>
ajout du call de fetch pour les détails de requêtes
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="81">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -127,7 +127,10 @@
     <t xml:space="preserve">Fix de l’api de Requêtes pour retourner les bon types de valeurs.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mise à jour de l’environnement de développement</t>
+    <t xml:space="preserve">Mise à jour de l’environnement de développement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout du lien à l’api pour l’affichage des détails de la requête.</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1024,9 +1027,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>117720</xdr:colOff>
+      <xdr:colOff>117360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1040,7 +1043,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2299680" cy="841320"/>
+          <a:ext cx="2299320" cy="840960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1066,9 +1069,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
+      <xdr:colOff>527040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212760</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1082,7 +1085,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401920" cy="784440"/>
+          <a:ext cx="2401560" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1108,9 +1111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
+      <xdr:colOff>527040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212760</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1124,7 +1127,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401920" cy="784440"/>
+          <a:ext cx="2401560" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1150,9 +1153,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
+      <xdr:colOff>527040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212760</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1166,7 +1169,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401920" cy="784440"/>
+          <a:ext cx="2401560" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1192,9 +1195,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
+      <xdr:colOff>527040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212760</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1208,7 +1211,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401920" cy="784440"/>
+          <a:ext cx="2401560" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1234,9 +1237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
+      <xdr:colOff>527040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212760</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1250,7 +1253,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401920" cy="784440"/>
+          <a:ext cx="2401560" cy="784080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1273,7 +1276,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1358,7 +1361,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1424,10 +1427,18 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="n">
+        <v>31</v>
+      </c>
+      <c r="C14" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33"/>
@@ -4183,7 +4194,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4232,10 +4243,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4260,13 +4271,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4290,13 +4301,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4321,7 +4332,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4338,7 +4349,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4355,10 +4366,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4377,10 +4388,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4396,10 +4407,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4415,10 +4426,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4434,10 +4445,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4453,10 +4464,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4472,10 +4483,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4491,10 +4502,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4510,10 +4521,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4529,10 +4540,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4548,10 +4559,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4567,10 +4578,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4586,10 +4597,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4605,10 +4616,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4624,10 +4635,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4655,7 +4666,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4803,7 +4814,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4864,13 +4875,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4895,10 +4906,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4911,10 +4922,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -4927,10 +4938,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4949,10 +4960,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4968,10 +4979,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4987,10 +4998,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5006,10 +5017,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5025,10 +5036,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5044,10 +5055,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5063,10 +5074,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5082,10 +5093,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5101,10 +5112,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5120,10 +5131,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5139,10 +5150,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5158,10 +5169,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5177,10 +5188,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5196,10 +5207,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5227,7 +5238,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5373,7 +5384,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5434,13 +5445,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5465,10 +5476,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5481,10 +5492,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5497,10 +5508,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5519,10 +5530,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5538,10 +5549,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5557,10 +5568,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5576,10 +5587,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5595,10 +5606,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5614,10 +5625,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5633,10 +5644,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5652,10 +5663,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5671,10 +5682,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5690,10 +5701,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5709,10 +5720,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5728,10 +5739,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5747,10 +5758,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5766,10 +5777,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5797,7 +5808,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -5943,7 +5954,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6004,13 +6015,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6035,10 +6046,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6051,10 +6062,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6067,10 +6078,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6089,10 +6100,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6108,10 +6119,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6127,10 +6138,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6146,10 +6157,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6165,10 +6176,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6184,10 +6195,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6203,10 +6214,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6222,10 +6233,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6241,10 +6252,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6260,10 +6271,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6279,10 +6290,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6298,10 +6309,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6317,10 +6328,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6336,10 +6347,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6367,7 +6378,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6513,7 +6524,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6574,13 +6585,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6605,10 +6616,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6621,10 +6632,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6637,10 +6648,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6659,10 +6670,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6678,10 +6689,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6697,10 +6708,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6716,10 +6727,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6735,10 +6746,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6754,10 +6765,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6773,10 +6784,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6792,10 +6803,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6811,10 +6822,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6830,10 +6841,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6849,10 +6860,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6868,10 +6879,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6887,10 +6898,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6906,10 +6917,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6937,7 +6948,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7066,7 +7077,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7074,7 +7085,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7082,7 +7093,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7090,7 +7101,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7098,7 +7109,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7106,7 +7117,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
40 - lien a l'api pour la création d'un nouveau Dossier
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ajout du lien à l’api pour l’affichage des détails de la requête.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07-02-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lien à l’api pour la création de dossier.</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1027,9 +1033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>117360</xdr:colOff>
+      <xdr:colOff>117000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1043,7 +1049,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2299320" cy="840960"/>
+          <a:ext cx="2298960" cy="840600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1069,9 +1075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>526680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212400</xdr:rowOff>
+      <xdr:rowOff>212040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1085,7 +1091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401560" cy="784080"/>
+          <a:ext cx="2401200" cy="783720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1111,9 +1117,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>526680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212400</xdr:rowOff>
+      <xdr:rowOff>212040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1127,7 +1133,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401560" cy="784080"/>
+          <a:ext cx="2401200" cy="783720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1153,9 +1159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>526680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212400</xdr:rowOff>
+      <xdr:rowOff>212040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1169,7 +1175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401560" cy="784080"/>
+          <a:ext cx="2401200" cy="783720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1195,9 +1201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>526680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212400</xdr:rowOff>
+      <xdr:rowOff>212040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1211,7 +1217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401560" cy="784080"/>
+          <a:ext cx="2401200" cy="783720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1237,9 +1243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
+      <xdr:colOff>526680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212400</xdr:rowOff>
+      <xdr:rowOff>212040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1253,7 +1259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401560" cy="784080"/>
+          <a:ext cx="2401200" cy="783720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,7 +1282,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1361,7 +1367,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1447,10 +1453,18 @@
       <c r="D15" s="34"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="34"/>
+      <c r="A16" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="34" t="n">
+        <v>40</v>
+      </c>
+      <c r="C16" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33"/>
@@ -4194,7 +4208,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4243,10 +4257,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4271,13 +4285,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4301,13 +4315,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4332,7 +4346,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4349,7 +4363,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4366,10 +4380,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4388,10 +4402,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4407,10 +4421,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4426,10 +4440,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4445,10 +4459,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4464,10 +4478,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4483,10 +4497,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4502,10 +4516,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4521,10 +4535,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4540,10 +4554,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4559,10 +4573,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4578,10 +4592,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4597,10 +4611,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4616,10 +4630,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4635,10 +4649,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4666,7 +4680,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4814,7 +4828,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4875,13 +4889,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4906,10 +4920,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4922,10 +4936,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -4938,10 +4952,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4960,10 +4974,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4979,10 +4993,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4998,10 +5012,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5017,10 +5031,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5036,10 +5050,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5055,10 +5069,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5074,10 +5088,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5093,10 +5107,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5112,10 +5126,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5131,10 +5145,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5150,10 +5164,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5169,10 +5183,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5188,10 +5202,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5207,10 +5221,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5238,7 +5252,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5384,7 +5398,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5445,13 +5459,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5476,10 +5490,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5492,10 +5506,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5508,10 +5522,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5530,10 +5544,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5549,10 +5563,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5568,10 +5582,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5587,10 +5601,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5606,10 +5620,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5625,10 +5639,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5644,10 +5658,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5663,10 +5677,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5682,10 +5696,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5701,10 +5715,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5720,10 +5734,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5739,10 +5753,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5758,10 +5772,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5777,10 +5791,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5808,7 +5822,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -5954,7 +5968,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6015,13 +6029,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6046,10 +6060,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6062,10 +6076,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6078,10 +6092,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6100,10 +6114,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6119,10 +6133,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6138,10 +6152,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6157,10 +6171,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6176,10 +6190,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6195,10 +6209,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6214,10 +6228,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6233,10 +6247,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6252,10 +6266,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6271,10 +6285,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6290,10 +6304,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6309,10 +6323,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6328,10 +6342,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6347,10 +6361,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6378,7 +6392,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6524,7 +6538,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6585,13 +6599,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6616,10 +6630,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6632,10 +6646,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6648,10 +6662,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6670,10 +6684,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6689,10 +6703,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6708,10 +6722,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6727,10 +6741,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6746,10 +6760,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6765,10 +6779,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6784,10 +6798,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6803,10 +6817,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6822,10 +6836,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6841,10 +6855,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6860,10 +6874,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6879,10 +6893,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6898,10 +6912,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6917,10 +6931,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6948,7 +6962,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7077,7 +7091,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7085,7 +7099,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7093,7 +7107,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7101,7 +7115,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7109,7 +7123,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7117,7 +7131,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
31 - get api pour le détails de requêtes
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="83">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -1033,9 +1033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>117000</xdr:colOff>
+      <xdr:colOff>116640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1049,7 +1049,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2298960" cy="840600"/>
+          <a:ext cx="2298600" cy="840240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1075,9 +1075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,7 +1091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401200" cy="783720"/>
+          <a:ext cx="2400840" cy="783360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,9 +1117,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1133,7 +1133,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401200" cy="783720"/>
+          <a:ext cx="2400840" cy="783360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1159,9 +1159,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1175,7 +1175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401200" cy="783720"/>
+          <a:ext cx="2400840" cy="783360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1201,9 +1201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,7 +1217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401200" cy="783720"/>
+          <a:ext cx="2400840" cy="783360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,9 +1243,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526680</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>212040</xdr:rowOff>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1259,7 +1259,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2401200" cy="783720"/>
+          <a:ext cx="2400840" cy="783360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1282,7 +1282,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>12</v>
+        <v>13.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1467,10 +1467,18 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="34"/>
+      <c r="A17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="34" t="n">
+        <v>31</v>
+      </c>
+      <c r="C17" s="35" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33"/>

</xml_diff>

<commit_message>
affiche un message d'erreur s'il est impossible de se connecter au serveur pour réessayer
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="85">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lien à l’api pour la création de dossier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-02-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion d’erreur lors de l’appelle à l’api pour la liste de dossiers</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1033,9 +1039,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>116640</xdr:colOff>
+      <xdr:colOff>116280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1049,7 +1055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2298600" cy="840240"/>
+          <a:ext cx="2298240" cy="839880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1075,9 +1081,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>211680</xdr:rowOff>
+      <xdr:rowOff>211320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1091,7 +1097,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400840" cy="783360"/>
+          <a:ext cx="2400480" cy="783000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,9 +1123,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>211680</xdr:rowOff>
+      <xdr:rowOff>211320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1133,7 +1139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400840" cy="783360"/>
+          <a:ext cx="2400480" cy="783000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1159,9 +1165,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>211680</xdr:rowOff>
+      <xdr:rowOff>211320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1175,7 +1181,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400840" cy="783360"/>
+          <a:ext cx="2400480" cy="783000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1201,9 +1207,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>211680</xdr:rowOff>
+      <xdr:rowOff>211320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,7 +1223,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400840" cy="783360"/>
+          <a:ext cx="2400480" cy="783000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,9 +1249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>211680</xdr:rowOff>
+      <xdr:rowOff>211320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1259,7 +1265,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2400840" cy="783360"/>
+          <a:ext cx="2400480" cy="783000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1282,7 +1288,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,7 +1373,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1487,10 +1493,18 @@
       <c r="D18" s="34"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="34"/>
+      <c r="A19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33"/>
@@ -4216,7 +4230,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4265,10 +4279,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4293,13 +4307,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4323,13 +4337,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4354,7 +4368,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4371,7 +4385,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4388,10 +4402,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4410,10 +4424,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4429,10 +4443,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4448,10 +4462,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4467,10 +4481,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4486,10 +4500,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4505,10 +4519,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4524,10 +4538,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4543,10 +4557,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4562,10 +4576,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4581,10 +4595,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4600,10 +4614,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4619,10 +4633,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4638,10 +4652,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4657,10 +4671,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4688,7 +4702,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4836,7 +4850,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4897,13 +4911,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4928,10 +4942,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4944,10 +4958,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -4960,10 +4974,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4982,10 +4996,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5001,10 +5015,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5020,10 +5034,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5039,10 +5053,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5058,10 +5072,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5077,10 +5091,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5096,10 +5110,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5115,10 +5129,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5134,10 +5148,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5153,10 +5167,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5172,10 +5186,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5191,10 +5205,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5210,10 +5224,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5229,10 +5243,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5260,7 +5274,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5406,7 +5420,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5467,13 +5481,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5498,10 +5512,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5514,10 +5528,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5530,10 +5544,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5552,10 +5566,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5571,10 +5585,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5590,10 +5604,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5609,10 +5623,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5628,10 +5642,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5647,10 +5661,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5666,10 +5680,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5685,10 +5699,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5704,10 +5718,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5723,10 +5737,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5742,10 +5756,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5761,10 +5775,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5780,10 +5794,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5799,10 +5813,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5830,7 +5844,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -5976,7 +5990,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6037,13 +6051,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6068,10 +6082,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6084,10 +6098,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6100,10 +6114,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6122,10 +6136,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6141,10 +6155,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6160,10 +6174,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6179,10 +6193,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6198,10 +6212,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6217,10 +6231,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6236,10 +6250,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6255,10 +6269,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6274,10 +6288,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6293,10 +6307,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6312,10 +6326,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6331,10 +6345,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6350,10 +6364,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6369,10 +6383,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6400,7 +6414,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6546,7 +6560,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6607,13 +6621,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6638,10 +6652,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6654,10 +6668,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6670,10 +6684,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6692,10 +6706,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6711,10 +6725,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6730,10 +6744,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6749,10 +6763,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6768,10 +6782,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6787,10 +6801,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6806,10 +6820,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6825,10 +6839,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6844,10 +6858,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6863,10 +6877,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6882,10 +6896,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6901,10 +6915,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6920,10 +6934,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6939,10 +6953,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6970,7 +6984,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7099,7 +7113,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7107,7 +7121,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7115,7 +7129,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7123,7 +7137,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7131,7 +7145,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7139,7 +7153,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
38 - validation frontend de la date de naissance dans la création de Dossier
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="88">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aide au développement de l’affichage des requêtes d’analyse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage d’erreur de validation async dans la création de dossier.</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1379,7 +1382,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>17</v>
+        <v>19.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1541,10 +1544,18 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="34"/>
+      <c r="A22" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="34" t="n">
+        <v>38</v>
+      </c>
+      <c r="C22" s="35" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="33"/>
@@ -4252,7 +4263,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4301,10 +4312,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4329,13 +4340,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4359,13 +4370,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4390,7 +4401,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4407,7 +4418,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4424,10 +4435,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4446,10 +4457,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4465,10 +4476,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4484,10 +4495,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4503,10 +4514,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4522,10 +4533,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4541,10 +4552,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4560,10 +4571,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4579,10 +4590,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4598,10 +4609,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4617,10 +4628,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4636,10 +4647,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4655,10 +4666,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4674,10 +4685,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4693,10 +4704,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4724,7 +4735,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4872,7 +4883,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4933,13 +4944,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4964,10 +4975,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4980,10 +4991,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -4996,10 +5007,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5018,10 +5029,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5037,10 +5048,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5056,10 +5067,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5075,10 +5086,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5094,10 +5105,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5113,10 +5124,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5132,10 +5143,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5151,10 +5162,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5170,10 +5181,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5189,10 +5200,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5208,10 +5219,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5227,10 +5238,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5246,10 +5257,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5265,10 +5276,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5296,7 +5307,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5442,7 +5453,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5503,13 +5514,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5534,10 +5545,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5550,10 +5561,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5566,10 +5577,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5588,10 +5599,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5607,10 +5618,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5626,10 +5637,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5645,10 +5656,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5664,10 +5675,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5683,10 +5694,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5702,10 +5713,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5721,10 +5732,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5740,10 +5751,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5759,10 +5770,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5778,10 +5789,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5797,10 +5808,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5816,10 +5827,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5835,10 +5846,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5866,7 +5877,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6012,7 +6023,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6073,13 +6084,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6104,10 +6115,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6120,10 +6131,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6136,10 +6147,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6158,10 +6169,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6177,10 +6188,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6196,10 +6207,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6215,10 +6226,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6234,10 +6245,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6253,10 +6264,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6272,10 +6283,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6291,10 +6302,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6310,10 +6321,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6329,10 +6340,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6348,10 +6359,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6367,10 +6378,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6386,10 +6397,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6405,10 +6416,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6436,7 +6447,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6582,7 +6593,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6643,13 +6654,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6674,10 +6685,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6690,10 +6701,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6706,10 +6717,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6728,10 +6739,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6747,10 +6758,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6766,10 +6777,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6785,10 +6796,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6804,10 +6815,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6823,10 +6834,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6842,10 +6853,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6861,10 +6872,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6880,10 +6891,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6899,10 +6910,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6918,10 +6929,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6937,10 +6948,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6956,10 +6967,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6975,10 +6986,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -7006,7 +7017,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7135,7 +7146,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7143,7 +7154,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7151,7 +7162,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7159,7 +7170,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7167,7 +7178,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7175,7 +7186,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
changement de l'affichage de la date et du sexe dans les détails de dossiers
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="89">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Affichage d’erreur de validation async dans la création de dossier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-02-2023</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1048,9 +1051,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>115560</xdr:colOff>
+      <xdr:colOff>115200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1064,7 +1067,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2297520" cy="839160"/>
+          <a:ext cx="2297160" cy="838800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1090,9 +1093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>210240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1106,7 +1109,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399760" cy="782280"/>
+          <a:ext cx="2399400" cy="781920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1132,9 +1135,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>210240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1148,7 +1151,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399760" cy="782280"/>
+          <a:ext cx="2399400" cy="781920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1174,9 +1177,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>210240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1190,7 +1193,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399760" cy="782280"/>
+          <a:ext cx="2399400" cy="781920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1216,9 +1219,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>210240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1232,7 +1235,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399760" cy="782280"/>
+          <a:ext cx="2399400" cy="781920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1258,9 +1261,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210600</xdr:rowOff>
+      <xdr:rowOff>210240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1274,7 +1277,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399760" cy="782280"/>
+          <a:ext cx="2399400" cy="781920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1296,8 +1299,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,7 +1567,9 @@
       <c r="D23" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="33"/>
+      <c r="A24" s="33" t="s">
+        <v>25</v>
+      </c>
       <c r="B24" s="34"/>
       <c r="C24" s="35"/>
       <c r="D24" s="34"/>
@@ -4263,7 +4268,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4312,10 +4317,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4340,13 +4345,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4370,13 +4375,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4401,7 +4406,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4418,7 +4423,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4435,10 +4440,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4457,10 +4462,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4476,10 +4481,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4495,10 +4500,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4514,10 +4519,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4533,10 +4538,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4552,10 +4557,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4571,10 +4576,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4590,10 +4595,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4609,10 +4614,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4628,10 +4633,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4647,10 +4652,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4666,10 +4671,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4685,10 +4690,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4704,10 +4709,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4735,7 +4740,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4883,7 +4888,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4944,13 +4949,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4975,10 +4980,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4991,10 +4996,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5007,10 +5012,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5029,10 +5034,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5048,10 +5053,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5067,10 +5072,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5086,10 +5091,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5105,10 +5110,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5124,10 +5129,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5143,10 +5148,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5162,10 +5167,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5181,10 +5186,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5200,10 +5205,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5219,10 +5224,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5238,10 +5243,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5257,10 +5262,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5276,10 +5281,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5307,7 +5312,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5453,7 +5458,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5514,13 +5519,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5545,10 +5550,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5561,10 +5566,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5577,10 +5582,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5599,10 +5604,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5618,10 +5623,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5637,10 +5642,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5656,10 +5661,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5675,10 +5680,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5694,10 +5699,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5713,10 +5718,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5732,10 +5737,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5751,10 +5756,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5770,10 +5775,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5789,10 +5794,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5808,10 +5813,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5827,10 +5832,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5846,10 +5851,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5877,7 +5882,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6023,7 +6028,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6084,13 +6089,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6115,10 +6120,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6131,10 +6136,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6147,10 +6152,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6169,10 +6174,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6188,10 +6193,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6207,10 +6212,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6226,10 +6231,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6245,10 +6250,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6264,10 +6269,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6283,10 +6288,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6302,10 +6307,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6321,10 +6326,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6340,10 +6345,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6359,10 +6364,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6378,10 +6383,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6397,10 +6402,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6416,10 +6421,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6447,7 +6452,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6593,7 +6598,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6654,13 +6659,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6685,10 +6690,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6701,10 +6706,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6717,10 +6722,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6739,10 +6744,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6758,10 +6763,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6777,10 +6782,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6796,10 +6801,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6815,10 +6820,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6834,10 +6839,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6853,10 +6858,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6872,10 +6877,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6891,10 +6896,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6910,10 +6915,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6929,10 +6934,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6948,10 +6953,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6967,10 +6972,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6986,10 +6991,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -7017,7 +7022,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7146,7 +7151,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7154,7 +7159,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7162,7 +7167,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7170,7 +7175,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7178,7 +7183,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7186,7 +7191,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
separation de la date et de l'heure dans l'affichage de détails d'une requête
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="91">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">12-02-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement de l’affichage dans les details de dossiers pour ne pas voir l’heure dans la date de naissance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement de l’affichage du sexe dans les details de dossiers pour ne pas être un chiffre</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1300,13 +1306,13 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="76.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="82.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.44"/>
   </cols>
   <sheetData>
@@ -1385,7 +1391,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>19.5</v>
+        <v>20.25</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1570,15 +1576,29 @@
       <c r="A24" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="33"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="34"/>
+      <c r="A25" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="35" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="33"/>
@@ -4268,7 +4288,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4317,10 +4337,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4345,13 +4365,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4375,13 +4395,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4406,7 +4426,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4423,7 +4443,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4440,10 +4460,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4462,10 +4482,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4481,10 +4501,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4500,10 +4520,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4519,10 +4539,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4538,10 +4558,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4557,10 +4577,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4576,10 +4596,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4595,10 +4615,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4614,10 +4634,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4633,10 +4653,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4652,10 +4672,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4671,10 +4691,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E26" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4690,10 +4710,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E27" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4709,10 +4729,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E28" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4740,7 +4760,7 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -4888,7 +4908,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4949,13 +4969,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -4980,10 +5000,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -4996,10 +5016,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5012,10 +5032,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5034,10 +5054,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5053,10 +5073,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5072,10 +5092,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5091,10 +5111,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5110,10 +5130,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5129,10 +5149,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5148,10 +5168,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5167,10 +5187,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5186,10 +5206,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5205,10 +5225,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5224,10 +5244,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5243,10 +5263,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5262,10 +5282,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5281,10 +5301,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5312,7 +5332,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
@@ -5458,7 +5478,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5519,13 +5539,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5550,10 +5570,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5566,10 +5586,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5582,10 +5602,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5604,10 +5624,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5623,10 +5643,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5642,10 +5662,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5661,10 +5681,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5680,10 +5700,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5699,10 +5719,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5718,10 +5738,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5737,10 +5757,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5756,10 +5776,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5775,10 +5795,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5794,10 +5814,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5813,10 +5833,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5832,10 +5852,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5851,10 +5871,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5882,7 +5902,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6028,7 +6048,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6089,13 +6109,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6120,10 +6140,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6136,10 +6156,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6152,10 +6172,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6174,10 +6194,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6193,10 +6213,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6212,10 +6232,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6231,10 +6251,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6250,10 +6270,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6269,10 +6289,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6288,10 +6308,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6307,10 +6327,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6326,10 +6346,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6345,10 +6365,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6364,10 +6384,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6383,10 +6403,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6402,10 +6422,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6421,10 +6441,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6452,7 +6472,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -6598,7 +6618,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6659,13 +6679,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6690,10 +6710,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6706,10 +6726,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6722,10 +6742,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6744,10 +6764,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6763,10 +6783,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6782,10 +6802,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6801,10 +6821,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6820,10 +6840,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6839,10 +6859,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6858,10 +6878,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6877,10 +6897,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6896,10 +6916,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6915,10 +6935,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6934,10 +6954,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6953,10 +6973,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6972,10 +6992,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6991,10 +7011,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -7022,7 +7042,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
@@ -7151,7 +7171,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7159,7 +7179,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7167,7 +7187,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7175,7 +7195,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7183,7 +7203,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7191,7 +7211,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
temps et commentaires de coéquipiers
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="97">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changement de l’affichage du sexe dans les details de dossiers pour ne pas être un chiffre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement de l’affichage de la date de prélevement dans les details de requêtes.</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -296,6 +299,9 @@
     <t xml:space="preserve">Commentaires:</t>
   </si>
   <si>
+    <t xml:space="preserve">Je prends souvent trop de place ne laissant pas tout le temps l’opinion des autres être écouté. Je commence souvent à déranger en parlant d’autre sujets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 3</t>
   </si>
   <si>
@@ -353,6 +359,9 @@
     <t xml:space="preserve">A eu à cœur la cohérence de l'ensemble du travail final.</t>
   </si>
   <si>
+    <t xml:space="preserve">Karl a bien travaillé et demande souvent l’opinions des autres afin de garder une bonne cohérence dans le projet. Cepandnat il semble parfois avoir de la misère à faire les choix par lui-même.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 4</t>
   </si>
   <si>
@@ -365,6 +374,9 @@
     <t xml:space="preserve">Garceau</t>
   </si>
   <si>
+    <t xml:space="preserve">Louis a majoritairement bien travailler, mais certain de ces développement ne suivait pas ce qui avait été établit. Cela peut être expliqué par un manque de compréhension entre lui et les autres membres de l’équipe. Il a parfois de la difficulté à demander aux autres s’il a bien compris</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coéquipier 3</t>
   </si>
   <si>
@@ -374,6 +386,9 @@
     <t xml:space="preserve">Belval</t>
   </si>
   <si>
+    <t xml:space="preserve">Jean-Philippe a super bien bien travailler, cependant il n’a pas vraiment fait de révision du travail des autres.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 5</t>
   </si>
   <si>
@@ -384,6 +399,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aubin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxime a très bien travaillé, mais n’est pas tout le temps actif lors des conversations d’équipes.</t>
   </si>
   <si>
     <t xml:space="preserve"> - Sélectionnez -</t>
@@ -725,7 +743,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -942,7 +960,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -954,8 +972,8 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -969,10 +987,6 @@
     <xf numFmtId="166" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1305,8 +1319,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1391,7 +1405,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>20.25</v>
+        <v>20.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1601,10 +1615,18 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="34"/>
+      <c r="A26" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="35" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="33"/>
@@ -4261,7 +4283,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4288,7 +4310,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4337,10 +4359,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4365,13 +4387,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4395,13 +4417,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4426,7 +4448,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4443,7 +4465,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4460,18 +4482,17 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D14,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="55" t="n">
         <f aca="false">IFERROR(SUM(E14:E28),"Autoévaluation à faire")</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G14" s="55"/>
       <c r="H14" s="55"/>
@@ -4482,14 +4503,13 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D15,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15" s="55"/>
       <c r="G15" s="55"/>
@@ -4501,10 +4521,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4520,10 +4540,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4539,14 +4559,13 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D18,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="55"/>
       <c r="G18" s="55"/>
@@ -4558,14 +4577,13 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D19,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="55"/>
       <c r="G19" s="55"/>
@@ -4577,10 +4595,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4596,10 +4614,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4615,14 +4633,13 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D22,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
@@ -4634,14 +4651,13 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D23,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" s="55"/>
       <c r="G23" s="55"/>
@@ -4653,10 +4669,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4672,14 +4688,13 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="55"/>
       <c r="G25" s="55"/>
@@ -4691,14 +4706,13 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E26" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D26,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26" s="55"/>
       <c r="G26" s="55"/>
@@ -4710,13 +4724,12 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E27" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D27,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F27" s="55"/>
@@ -4729,14 +4742,13 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E28" s="54" t="n">
-        <f aca="false">VLOOKUP(Évaluateur!D28,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F28" s="55"/>
       <c r="G28" s="55"/>
@@ -4760,9 +4772,11 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="57"/>
+        <v>56</v>
+      </c>
+      <c r="D30" s="57" t="s">
+        <v>57</v>
+      </c>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
       <c r="G30" s="57"/>
@@ -4881,7 +4895,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4908,7 +4922,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4969,13 +4983,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5000,10 +5014,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5016,10 +5030,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5032,18 +5046,17 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="60" t="n">
         <f aca="false">IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
@@ -5054,14 +5067,13 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="60"/>
       <c r="G12" s="60"/>
@@ -5073,14 +5085,13 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
@@ -5092,14 +5103,13 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
@@ -5111,10 +5121,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5130,10 +5140,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5149,14 +5159,13 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="60"/>
       <c r="G17" s="60"/>
@@ -5168,14 +5177,13 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -5187,14 +5195,13 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
@@ -5206,14 +5213,13 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -5225,14 +5231,13 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="60"/>
       <c r="G21" s="60"/>
@@ -5244,14 +5249,13 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60"/>
@@ -5263,14 +5267,13 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" s="60"/>
       <c r="G23" s="60"/>
@@ -5282,10 +5285,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5301,14 +5304,13 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 1'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
@@ -5332,14 +5334,16 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
+        <v>56</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
       <c r="J27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,8 +5454,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5478,7 +5482,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5539,13 +5543,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5570,10 +5574,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5586,10 +5590,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5602,18 +5606,17 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="60" t="n">
         <f aca="false">IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
@@ -5624,14 +5627,13 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="60"/>
       <c r="G12" s="60"/>
@@ -5643,14 +5645,13 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
@@ -5662,14 +5663,13 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
@@ -5681,14 +5681,13 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="60"/>
       <c r="G15" s="60"/>
@@ -5700,13 +5699,12 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F16" s="60"/>
@@ -5719,14 +5717,13 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="60"/>
       <c r="G17" s="60"/>
@@ -5738,14 +5735,13 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -5757,14 +5753,13 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
@@ -5776,14 +5771,13 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -5795,14 +5789,13 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="60"/>
       <c r="G21" s="60"/>
@@ -5814,14 +5807,13 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60"/>
@@ -5833,13 +5825,12 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F23" s="60"/>
@@ -5852,10 +5843,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5871,14 +5862,13 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 2'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
@@ -5902,9 +5892,11 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="57"/>
+        <v>56</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>82</v>
+      </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
       <c r="G27" s="57"/>
@@ -6020,8 +6012,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6048,7 +6040,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6109,13 +6101,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6140,10 +6132,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6156,10 +6148,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6172,18 +6164,17 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="60" t="n">
         <f aca="false">IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
@@ -6194,14 +6185,13 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="60"/>
       <c r="G12" s="60"/>
@@ -6213,14 +6203,13 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
@@ -6232,14 +6221,13 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
@@ -6251,14 +6239,13 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15" s="60"/>
       <c r="G15" s="60"/>
@@ -6270,14 +6257,13 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16" s="60"/>
       <c r="G16" s="60"/>
@@ -6289,14 +6275,13 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="60"/>
       <c r="G17" s="60"/>
@@ -6308,14 +6293,13 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -6327,14 +6311,13 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
@@ -6346,14 +6329,13 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -6365,14 +6347,13 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="60"/>
       <c r="G21" s="60"/>
@@ -6384,14 +6365,13 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60"/>
@@ -6403,14 +6383,13 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" s="60"/>
       <c r="G23" s="60"/>
@@ -6422,13 +6401,12 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F24" s="60"/>
@@ -6441,14 +6419,13 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 3'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
@@ -6472,9 +6449,11 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="57"/>
+        <v>56</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>86</v>
+      </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
       <c r="G27" s="57"/>
@@ -6590,8 +6569,8 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6618,7 +6597,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6679,13 +6658,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6710,10 +6689,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6726,10 +6705,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6742,18 +6721,17 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D11,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="60" t="n">
         <f aca="false">IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
@@ -6764,14 +6742,13 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D12,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="60"/>
       <c r="G12" s="60"/>
@@ -6783,13 +6760,12 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D13,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F13" s="60"/>
@@ -6802,14 +6778,13 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D14,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
@@ -6821,13 +6796,12 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
         <v>4</v>
       </c>
       <c r="F15" s="60"/>
@@ -6840,10 +6814,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6859,14 +6833,13 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D17,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="60"/>
       <c r="G17" s="60"/>
@@ -6878,14 +6851,13 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D18,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
@@ -6897,14 +6869,13 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D19,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="60"/>
       <c r="G19" s="60"/>
@@ -6916,14 +6887,13 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D20,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -6935,14 +6905,13 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D21,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="60"/>
       <c r="G21" s="60"/>
@@ -6954,14 +6923,13 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D22,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60"/>
@@ -6973,14 +6941,13 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D23,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" s="60"/>
       <c r="G23" s="60"/>
@@ -6992,14 +6959,13 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F24" s="60"/>
       <c r="G24" s="60"/>
@@ -7011,14 +6977,13 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" s="54" t="n">
-        <f aca="false">VLOOKUP('Coéquipier 4'!D25,Menu!$B$4:$C$8,2,FALSE())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
@@ -7042,9 +7007,11 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="57"/>
+        <v>56</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>91</v>
+      </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
       <c r="G27" s="57"/>
@@ -7171,7 +7138,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7179,7 +7146,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7187,7 +7154,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7195,7 +7162,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7203,7 +7170,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7211,7 +7178,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
l'affichage de la date et du sexe dans tout les endroits qui prenne le dossier à partir du FolderDetails devrait être chillax
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Temps" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="98">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changement de l’affichage de la date de prélevement dans les details de requêtes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactorisation du fetch pour l’affichage de détails de dossier pour avoir des valeurs spécifique à l’affichage</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1071,9 +1074,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>115200</xdr:colOff>
+      <xdr:colOff>114840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1087,7 +1090,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2297160" cy="838800"/>
+          <a:ext cx="2296800" cy="838440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1113,9 +1116,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210240</xdr:rowOff>
+      <xdr:rowOff>209880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1129,7 +1132,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399400" cy="781920"/>
+          <a:ext cx="2399040" cy="781560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1155,9 +1158,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210240</xdr:rowOff>
+      <xdr:rowOff>209880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1171,7 +1174,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399400" cy="781920"/>
+          <a:ext cx="2399040" cy="781560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1197,9 +1200,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210240</xdr:rowOff>
+      <xdr:rowOff>209880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1213,7 +1216,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399400" cy="781920"/>
+          <a:ext cx="2399040" cy="781560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1239,9 +1242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210240</xdr:rowOff>
+      <xdr:rowOff>209880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1255,7 +1258,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399400" cy="781920"/>
+          <a:ext cx="2399040" cy="781560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1281,9 +1284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>524520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>210240</xdr:rowOff>
+      <xdr:rowOff>209880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1297,7 +1300,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2399400" cy="781920"/>
+          <a:ext cx="2399040" cy="781560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1319,14 +1322,14 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="82.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="84.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.44"/>
   </cols>
   <sheetData>
@@ -1405,7 +1408,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>20.5</v>
+        <v>21</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1629,10 +1632,18 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="34"/>
+      <c r="A27" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="33"/>
@@ -4310,7 +4321,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4359,10 +4370,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4387,13 +4398,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4417,13 +4428,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4448,7 +4459,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4465,7 +4476,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4482,10 +4493,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -4503,10 +4514,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -4521,10 +4532,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4540,10 +4551,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4559,10 +4570,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -4577,10 +4588,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -4595,10 +4606,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4614,10 +4625,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4633,10 +4644,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>3</v>
@@ -4651,10 +4662,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>3</v>
@@ -4669,10 +4680,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4688,10 +4699,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -4706,10 +4717,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26" s="54" t="n">
         <v>5</v>
@@ -4724,10 +4735,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E27" s="54" t="n">
         <v>4</v>
@@ -4742,10 +4753,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E28" s="54" t="n">
         <v>5</v>
@@ -4772,10 +4783,10 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D30" s="57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
@@ -4922,7 +4933,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4983,13 +4994,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5014,10 +5025,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5030,10 +5041,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5046,10 +5057,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5067,10 +5078,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5085,10 +5096,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5103,10 +5114,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5121,10 +5132,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5140,10 +5151,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5159,10 +5170,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5177,10 +5188,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5195,10 +5206,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5213,10 +5224,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5231,10 +5242,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5249,10 +5260,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5267,10 +5278,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -5285,10 +5296,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5304,10 +5315,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5334,10 +5345,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -5482,7 +5493,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5543,13 +5554,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5574,10 +5585,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5590,10 +5601,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5606,10 +5617,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5627,10 +5638,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5645,10 +5656,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5663,10 +5674,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5681,10 +5692,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>3</v>
@@ -5699,10 +5710,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>4</v>
@@ -5717,10 +5728,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5735,10 +5746,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5753,10 +5764,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5771,10 +5782,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5789,10 +5800,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5807,10 +5818,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5825,10 +5836,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>4</v>
@@ -5843,10 +5854,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5862,10 +5873,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5892,10 +5903,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6040,7 +6051,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6101,13 +6112,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6132,10 +6143,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6148,10 +6159,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6164,10 +6175,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6185,10 +6196,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6203,10 +6214,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -6221,10 +6232,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6239,10 +6250,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -6257,10 +6268,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>5</v>
@@ -6275,10 +6286,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6293,10 +6304,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6311,10 +6322,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6329,10 +6340,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6347,10 +6358,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6365,10 +6376,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6383,10 +6394,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6401,10 +6412,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>4</v>
@@ -6419,10 +6430,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -6449,10 +6460,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6569,7 +6580,7 @@
   </sheetPr>
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -6597,7 +6608,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6658,13 +6669,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6689,10 +6700,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6705,10 +6716,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6721,10 +6732,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6742,10 +6753,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6760,10 +6771,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>4</v>
@@ -6778,10 +6789,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6796,10 +6807,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>4</v>
@@ -6814,10 +6825,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6833,10 +6844,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6851,10 +6862,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6869,10 +6880,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6887,10 +6898,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6905,10 +6916,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6923,10 +6934,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6941,10 +6952,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6959,10 +6970,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>5</v>
@@ -6977,10 +6988,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -7007,10 +7018,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -7138,7 +7149,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7146,7 +7157,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7154,7 +7165,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7162,7 +7173,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7170,7 +7181,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7178,7 +7189,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
mes styles marchent po :(
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="99">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Refactorisation du fetch pour l’affichage de détails de dossier pour avoir des valeurs spécifique à l’affichage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement de style des bouttons de la liste de requêtes</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1322,8 +1325,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1408,7 +1411,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>21</v>
+        <v>21.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1646,10 +1649,18 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="34"/>
+      <c r="A28" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="33"/>
@@ -4321,7 +4332,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4370,10 +4381,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4398,13 +4409,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4428,13 +4439,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4459,7 +4470,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4476,7 +4487,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4493,10 +4504,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -4514,10 +4525,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -4532,10 +4543,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4551,10 +4562,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4570,10 +4581,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -4588,10 +4599,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -4606,10 +4617,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4625,10 +4636,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4644,10 +4655,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>3</v>
@@ -4662,10 +4673,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>3</v>
@@ -4680,10 +4691,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4699,10 +4710,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -4717,10 +4728,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E26" s="54" t="n">
         <v>5</v>
@@ -4735,10 +4746,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E27" s="54" t="n">
         <v>4</v>
@@ -4753,10 +4764,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E28" s="54" t="n">
         <v>5</v>
@@ -4783,10 +4794,10 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D30" s="57" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
@@ -4933,7 +4944,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4994,13 +5005,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5025,10 +5036,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5041,10 +5052,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5057,10 +5068,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5078,10 +5089,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5096,10 +5107,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5114,10 +5125,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5132,10 +5143,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5151,10 +5162,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5170,10 +5181,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5188,10 +5199,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5206,10 +5217,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5224,10 +5235,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5242,10 +5253,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5260,10 +5271,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5278,10 +5289,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -5296,10 +5307,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5315,10 +5326,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5345,10 +5356,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -5493,7 +5504,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5554,13 +5565,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5585,10 +5596,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5601,10 +5612,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5617,10 +5628,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5638,10 +5649,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5656,10 +5667,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5674,10 +5685,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5692,10 +5703,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>3</v>
@@ -5710,10 +5721,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>4</v>
@@ -5728,10 +5739,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5746,10 +5757,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5764,10 +5775,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5782,10 +5793,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5800,10 +5811,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5818,10 +5829,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5836,10 +5847,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>4</v>
@@ -5854,10 +5865,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5873,10 +5884,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5903,10 +5914,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6051,7 +6062,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6112,13 +6123,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6143,10 +6154,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6159,10 +6170,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6175,10 +6186,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6196,10 +6207,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6214,10 +6225,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -6232,10 +6243,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6250,10 +6261,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -6268,10 +6279,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>5</v>
@@ -6286,10 +6297,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6304,10 +6315,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6322,10 +6333,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6340,10 +6351,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6358,10 +6369,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6376,10 +6387,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6394,10 +6405,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6412,10 +6423,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>4</v>
@@ -6430,10 +6441,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -6460,10 +6471,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6608,7 +6619,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6669,13 +6680,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6700,10 +6711,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6716,10 +6727,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6732,10 +6743,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6753,10 +6764,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6771,10 +6782,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>4</v>
@@ -6789,10 +6800,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6807,10 +6818,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>4</v>
@@ -6825,10 +6836,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6844,10 +6855,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6862,10 +6873,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6880,10 +6891,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6898,10 +6909,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6916,10 +6927,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6934,10 +6945,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6952,10 +6963,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6970,10 +6981,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>5</v>
@@ -6988,10 +6999,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -7018,10 +7029,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -7149,7 +7160,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7157,7 +7168,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7165,7 +7176,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7173,7 +7184,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7181,7 +7192,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7189,7 +7200,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
better scaling for folderDetails view
</commit_message>
<xml_diff>
--- a/FichesTemps/VictorTurgeon-03.xlsx
+++ b/FichesTemps/VictorTurgeon-03.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="100">
   <si>
     <t xml:space="preserve">Feuille de temps - 420-6DY-HY Projets</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changement de style des bouttons de la liste de requêtes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustement au frontend de détails de dossier pour un affichage qui se formate mieu</t>
   </si>
   <si>
     <t xml:space="preserve">Fiche d'évaluation du travail d'équipe</t>
@@ -1325,8 +1328,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="C9" s="23" t="n">
         <f aca="false">SUM(C11:C462)</f>
-        <v>21.5</v>
+        <v>24.5</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -1580,7 +1583,7 @@
         <v>38</v>
       </c>
       <c r="C22" s="35" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>24</v>
@@ -1663,10 +1666,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="34"/>
+      <c r="A29" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="35" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="33"/>
@@ -4332,7 +4343,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -4381,10 +4392,10 @@
     <row r="6" customFormat="false" ht="138" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -4409,13 +4420,13 @@
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
@@ -4439,13 +4450,13 @@
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4470,7 +4481,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="51" t="str">
         <f aca="false">Temps!D6</f>
@@ -4487,7 +4498,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="47"/>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="51" t="str">
         <f aca="false">Temps!D7</f>
@@ -4504,10 +4515,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -4525,10 +4536,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -4543,10 +4554,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4562,10 +4573,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D17,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4581,10 +4592,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -4599,10 +4610,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -4617,10 +4628,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D20,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4636,10 +4647,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D21,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4655,10 +4666,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>3</v>
@@ -4673,10 +4684,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>3</v>
@@ -4691,10 +4702,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP(Évaluateur!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -4710,10 +4721,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -4728,10 +4739,10 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E26" s="54" t="n">
         <v>5</v>
@@ -4746,10 +4757,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E27" s="54" t="n">
         <v>4</v>
@@ -4764,10 +4775,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E28" s="54" t="n">
         <v>5</v>
@@ -4794,10 +4805,10 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D30" s="57" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E30" s="57"/>
       <c r="F30" s="57"/>
@@ -4944,7 +4955,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5005,13 +5016,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5036,10 +5047,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5052,10 +5063,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5068,10 +5079,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5089,10 +5100,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5107,10 +5118,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5125,10 +5136,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5143,10 +5154,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D15,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5162,10 +5173,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5181,10 +5192,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5199,10 +5210,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5217,10 +5228,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5235,10 +5246,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5253,10 +5264,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5271,10 +5282,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5289,10 +5300,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -5307,10 +5318,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 1'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5326,10 +5337,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5356,10 +5367,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -5504,7 +5515,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5565,13 +5576,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -5596,10 +5607,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -5612,10 +5623,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -5628,10 +5639,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -5649,10 +5660,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -5667,10 +5678,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -5685,10 +5696,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -5703,10 +5714,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>3</v>
@@ -5721,10 +5732,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>4</v>
@@ -5739,10 +5750,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -5757,10 +5768,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -5775,10 +5786,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -5793,10 +5804,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -5811,10 +5822,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -5829,10 +5840,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -5847,10 +5858,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>4</v>
@@ -5865,10 +5876,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 2'!D24,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -5884,10 +5895,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -5914,10 +5925,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6062,7 +6073,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6123,13 +6134,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6154,10 +6165,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6170,10 +6181,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6186,10 +6197,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6207,10 +6218,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6225,10 +6236,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>5</v>
@@ -6243,10 +6254,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6261,10 +6272,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>5</v>
@@ -6279,10 +6290,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="54" t="n">
         <v>5</v>
@@ -6297,10 +6308,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6315,10 +6326,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6333,10 +6344,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6351,10 +6362,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6369,10 +6380,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6387,10 +6398,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6405,10 +6416,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6423,10 +6434,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>4</v>
@@ -6441,10 +6452,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -6471,10 +6482,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -6619,7 +6630,7 @@
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6680,13 +6691,13 @@
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
@@ -6711,10 +6722,10 @@
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="59"/>
@@ -6727,10 +6738,10 @@
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -6743,10 +6754,10 @@
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="54" t="n">
         <v>5</v>
@@ -6764,10 +6775,10 @@
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="54" t="n">
         <v>5</v>
@@ -6782,10 +6793,10 @@
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="54" t="n">
         <v>4</v>
@@ -6800,10 +6811,10 @@
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" s="54" t="n">
         <v>5</v>
@@ -6818,10 +6829,10 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="54" t="n">
         <v>4</v>
@@ -6836,10 +6847,10 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E16" s="54" t="n">
         <f aca="false">VLOOKUP('Coéquipier 4'!D16,Menu!$B$4:$C$8,2,FALSE())</f>
@@ -6855,10 +6866,10 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="54" t="n">
         <v>5</v>
@@ -6873,10 +6884,10 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="54" t="n">
         <v>5</v>
@@ -6891,10 +6902,10 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="54" t="n">
         <v>5</v>
@@ -6909,10 +6920,10 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="54" t="n">
         <v>5</v>
@@ -6927,10 +6938,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="54" t="n">
         <v>5</v>
@@ -6945,10 +6956,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="54" t="n">
         <v>5</v>
@@ -6963,10 +6974,10 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="54" t="n">
         <v>5</v>
@@ -6981,10 +6992,10 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E24" s="54" t="n">
         <v>5</v>
@@ -6999,10 +7010,10 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E25" s="54" t="n">
         <v>5</v>
@@ -7029,10 +7040,10 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="56" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E27" s="57"/>
       <c r="F27" s="57"/>
@@ -7160,7 +7171,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -7168,7 +7179,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
@@ -7176,7 +7187,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -7184,7 +7195,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>3</v>
@@ -7192,7 +7203,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>4</v>
@@ -7200,7 +7211,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5</v>

</xml_diff>